<commit_message>
Added category and id generation
</commit_message>
<xml_diff>
--- a/input/link_table.xlsx
+++ b/input/link_table.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
   <si>
     <t xml:space="preserve">Numbers</t>
   </si>
@@ -28,10 +31,19 @@
     <t xml:space="preserve">Letters</t>
   </si>
   <si>
+    <t xml:space="preserve">/category</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
+    <t xml:space="preserve">/subcategory</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/id{x}-item{y}</t>
   </si>
 </sst>
 </file>
@@ -41,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +75,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,12 +126,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -125,6 +148,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -305,156 +388,171 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="8.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
+      <c r="B5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+      <c r="B7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>2</v>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>3</v>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>2</v>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>